<commit_message>
Vervang huidige risicoanalyse door gecorrigeerde risicoanalyse (#36)
* Vervang huidige risicoanalyse door gecorrigeerde risicoanalyse

* Beheer: Voeg gecorrigeerde excel risicoanalyse toe
</commit_message>
<xml_diff>
--- a/media/risicoanalyse-logboek-dataverwerkingen.xlsx
+++ b/media/risicoanalyse-logboek-dataverwerkingen.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC917D35-966B-42D4-BFCB-201A24324251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E07299D-D5A8-4F95-811C-E38154E3DAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13185" yWindow="-16425" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A6070C3D-585B-404B-8DE8-DADE5539500A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{A6070C3D-585B-404B-8DE8-DADE5539500A}"/>
   </bookViews>
   <sheets>
     <sheet name="Colofon" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="234">
   <si>
     <t>Component</t>
   </si>
@@ -1417,6 +1417,9 @@
 Handreiking data protection impact assessment (DPIA)
 Impact Assessment Mensenrechten en Algoritmes (IAMA)
 Cloudbeleid</t>
+  </si>
+  <si>
+    <t>Ongeautoriseerde toegang door onbevoegden (hackers/hosters)</t>
   </si>
 </sst>
 </file>
@@ -4776,13 +4779,13 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" customWidth="1"/>
-    <col min="2" max="2" width="105.6328125" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="105.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>49</v>
       </c>
@@ -4790,7 +4793,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>50</v>
       </c>
@@ -4798,7 +4801,7 @@
         <v>45796</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="25" t="s">
         <v>51</v>
       </c>
@@ -4806,7 +4809,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="25" t="s">
         <v>52</v>
       </c>
@@ -4814,7 +4817,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>59</v>
       </c>
@@ -4822,7 +4825,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>54</v>
       </c>
@@ -4830,7 +4833,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>55</v>
       </c>
@@ -4838,7 +4841,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>56</v>
       </c>
@@ -4846,11 +4849,11 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="15"/>
     </row>
-    <row r="11" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>57</v>
       </c>
@@ -4858,7 +4861,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
         <v>58</v>
       </c>
@@ -4882,33 +4885,33 @@
   <dimension ref="A1:U54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.81640625" style="29" customWidth="1"/>
-    <col min="3" max="3" width="62.08984375" style="2" customWidth="1"/>
-    <col min="4" max="6" width="6.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.81640625" style="2" customWidth="1"/>
-    <col min="8" max="10" width="8.81640625" style="2"/>
-    <col min="11" max="11" width="11.453125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="36.90625" style="31" customWidth="1"/>
-    <col min="13" max="13" width="21.08984375" style="31" customWidth="1"/>
-    <col min="14" max="14" width="20.36328125" style="31" customWidth="1"/>
-    <col min="15" max="15" width="18.1796875" style="31" customWidth="1"/>
-    <col min="16" max="16" width="19.81640625" style="31" customWidth="1"/>
-    <col min="17" max="17" width="18.54296875" style="31" customWidth="1"/>
-    <col min="18" max="18" width="53.90625" style="31" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.1796875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="19.1796875" style="2" customWidth="1"/>
-    <col min="22" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="1" width="14.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="29" customWidth="1"/>
+    <col min="3" max="3" width="62.109375" style="2" customWidth="1"/>
+    <col min="4" max="6" width="6.77734375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" style="2" customWidth="1"/>
+    <col min="8" max="10" width="8.77734375" style="2"/>
+    <col min="11" max="11" width="11.44140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="36.88671875" style="31" customWidth="1"/>
+    <col min="13" max="13" width="21.109375" style="31" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" style="31" customWidth="1"/>
+    <col min="15" max="15" width="18.21875" style="31" customWidth="1"/>
+    <col min="16" max="16" width="19.77734375" style="31" customWidth="1"/>
+    <col min="17" max="17" width="18.5546875" style="31" customWidth="1"/>
+    <col min="18" max="18" width="53.88671875" style="31" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.21875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="19.21875" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="81" t="s">
         <v>35</v>
       </c>
@@ -4933,8 +4936,8 @@
       <c r="T1" s="83"/>
       <c r="U1" s="83"/>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:21" ht="30.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:21" ht="30.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="53" t="s">
         <v>0</v>
       </c>
@@ -4983,7 +4986,7 @@
       <c r="T3" s="80"/>
       <c r="U3" s="80"/>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="57"/>
       <c r="B4" s="58"/>
       <c r="C4" s="59"/>
@@ -5034,7 +5037,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="48" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="70" t="s">
         <v>198</v>
       </c>
@@ -5112,7 +5115,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="57.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:21" ht="77.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>199</v>
       </c>
@@ -5188,7 +5191,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="32" t="s">
         <v>200</v>
       </c>
@@ -5264,7 +5267,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
         <v>202</v>
       </c>
@@ -5340,7 +5343,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="57.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:21" ht="77.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="70" t="s">
         <v>201</v>
       </c>
@@ -5416,7 +5419,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:21" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>203</v>
       </c>
@@ -5492,7 +5495,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="57.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:21" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
       <c r="B11" s="78">
         <v>7</v>
@@ -5566,7 +5569,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="57.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:21" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12"/>
       <c r="B12" s="78">
         <v>8</v>
@@ -5640,7 +5643,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="57.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:21" ht="67.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12"/>
       <c r="B13" s="78">
         <v>9</v>
@@ -5714,14 +5717,16 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="118.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:21" ht="118.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>204</v>
       </c>
       <c r="B14" s="78">
         <v>10</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>233</v>
+      </c>
       <c r="D14" s="33" t="s">
         <v>15</v>
       </c>
@@ -5788,7 +5793,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="114.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:21" ht="135" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12"/>
       <c r="B15" s="78">
         <v>11</v>
@@ -5862,7 +5867,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="114.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:21" ht="135" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12"/>
       <c r="B16" s="78">
         <v>12</v>
@@ -5936,7 +5941,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>205</v>
       </c>
@@ -6012,7 +6017,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12"/>
       <c r="B18" s="78">
         <v>14</v>
@@ -6088,7 +6093,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:21" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12"/>
       <c r="B19" s="78">
         <v>15</v>
@@ -6164,7 +6169,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>206</v>
       </c>
@@ -6240,7 +6245,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12"/>
       <c r="B21" s="78">
         <v>17</v>
@@ -6314,7 +6319,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="48" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>207</v>
       </c>
@@ -6390,7 +6395,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="48" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12"/>
       <c r="B23" s="78">
         <v>19</v>
@@ -6464,7 +6469,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="48" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12"/>
       <c r="B24" s="78">
         <v>20</v>
@@ -6538,7 +6543,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="48" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12"/>
       <c r="B25" s="78">
         <v>21</v>
@@ -6612,7 +6617,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="48" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12"/>
       <c r="B26" s="78">
         <v>22</v>
@@ -6686,7 +6691,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12"/>
       <c r="B27" s="78">
         <v>23</v>
@@ -6760,7 +6765,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>208</v>
       </c>
@@ -6836,7 +6841,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:21" ht="48.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12"/>
       <c r="B29" s="78">
         <v>25</v>
@@ -6912,7 +6917,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12"/>
       <c r="B30" s="78">
         <v>26</v>
@@ -6988,7 +6993,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12"/>
       <c r="B31" s="78">
         <v>27</v>
@@ -7064,7 +7069,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="48.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:21" ht="48.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>209</v>
       </c>
@@ -7140,7 +7145,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="64.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:21" ht="64.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>210</v>
       </c>
@@ -7216,7 +7221,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="61.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:21" ht="61.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
         <v>211</v>
       </c>
@@ -7292,7 +7297,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:21" ht="48.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>212</v>
       </c>
@@ -7370,7 +7375,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
         <v>213</v>
       </c>
@@ -7446,7 +7451,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12"/>
       <c r="B37" s="78">
         <v>33</v>
@@ -7520,7 +7525,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12"/>
       <c r="B38" s="78">
         <v>34</v>
@@ -7594,7 +7599,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12"/>
       <c r="B39" s="78">
         <v>35</v>
@@ -7668,7 +7673,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
         <v>214</v>
       </c>
@@ -7744,7 +7749,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="12"/>
       <c r="B41" s="78">
         <v>37</v>
@@ -7818,7 +7823,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="12"/>
       <c r="B42" s="78">
         <v>38</v>
@@ -7892,7 +7897,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="12"/>
       <c r="B43" s="78">
         <v>39</v>
@@ -7966,7 +7971,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:21" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="12"/>
       <c r="B44" s="78">
         <v>40</v>
@@ -8042,7 +8047,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
         <v>215</v>
       </c>
@@ -8118,7 +8123,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="12"/>
       <c r="B46" s="78">
         <v>42</v>
@@ -8192,7 +8197,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="76.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:21" ht="77.400000000000006" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="12" t="s">
         <v>216</v>
       </c>
@@ -8268,7 +8273,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:21" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="12"/>
       <c r="B48" s="78">
         <v>44</v>
@@ -8342,7 +8347,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="57.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="12"/>
       <c r="B49" s="78">
         <v>45</v>
@@ -8418,7 +8423,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:21" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>217</v>
       </c>
@@ -8496,7 +8501,7 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="12"/>
       <c r="B51" s="78">
         <v>47</v>
@@ -8572,8 +8577,8 @@
         <v>BBN1</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="87" t="s">
         <v>195</v>
       </c>
@@ -8594,7 +8599,7 @@
       <c r="P53" s="52"/>
       <c r="Q53" s="52"/>
     </row>
-    <row r="54" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="54" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A4:R34" xr:uid="{9686988F-52AC-49C6-A780-39E489F260FB}"/>
   <dataConsolidate/>
@@ -11409,24 +11414,24 @@
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1"/>
-    <col min="2" max="2" width="10.36328125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.81640625" style="1"/>
-    <col min="5" max="5" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" style="1"/>
-    <col min="7" max="7" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.81640625" style="1"/>
-    <col min="11" max="11" width="18.90625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.453125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="23.1796875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.81640625" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="8.77734375" style="1"/>
+    <col min="2" max="2" width="10.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.77734375" style="1"/>
+    <col min="5" max="5" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" style="1"/>
+    <col min="7" max="7" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="8.77734375" style="1"/>
+    <col min="11" max="11" width="18.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="23.21875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>34</v>
       </c>
@@ -11434,13 +11439,13 @@
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
     </row>
-    <row r="2" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
         <v>37</v>
       </c>
@@ -11451,7 +11456,7 @@
       <c r="J3" s="102"/>
       <c r="K3" s="103"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="67"/>
       <c r="E4" s="14"/>
       <c r="I4" s="21" t="s">
@@ -11464,7 +11469,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="68" t="s">
         <v>38</v>
       </c>
@@ -11472,7 +11477,7 @@
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
     </row>
-    <row r="6" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="69" t="s">
         <v>194</v>
       </c>
@@ -11486,7 +11491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I7" s="17" t="s">
         <v>14</v>
       </c>
@@ -11497,7 +11502,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I8" s="19" t="s">
         <v>13</v>
       </c>
@@ -11508,7 +11513,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -11517,7 +11522,7 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -11531,7 +11536,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="104" t="s">
@@ -11549,7 +11554,7 @@
       <c r="N14" s="97"/>
       <c r="O14" s="98"/>
     </row>
-    <row r="15" spans="1:15" ht="12.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="38" t="s">
@@ -11583,7 +11588,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="93" t="s">
         <v>90</v>
       </c>
@@ -11627,7 +11632,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="32.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="31.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="94"/>
       <c r="B17" s="37" t="s">
         <v>92</v>
@@ -11667,7 +11672,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="42.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="94"/>
       <c r="B18" s="37" t="s">
         <v>93</v>
@@ -11707,7 +11712,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="32.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" ht="31.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="94"/>
       <c r="B19" s="37" t="s">
         <v>94</v>
@@ -11747,7 +11752,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="32.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" ht="31.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="95"/>
       <c r="B20" s="37" t="s">
         <v>95</v>
@@ -11787,7 +11792,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.5">
       <c r="K22" s="71" t="s">
         <v>39</v>
       </c>
@@ -11795,7 +11800,7 @@
       <c r="M22"/>
       <c r="N22"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="99" t="s">
         <v>84</v>
       </c>
@@ -11813,7 +11818,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="29" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>48</v>
       </c>
@@ -11833,7 +11838,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="41" t="s">
         <v>100</v>
       </c>
@@ -11853,7 +11858,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="29" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="41" t="s">
         <v>99</v>
       </c>
@@ -11873,7 +11878,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="41" t="s">
         <v>98</v>
       </c>
@@ -11881,7 +11886,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
         <v>105</v>
       </c>
@@ -11889,7 +11894,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
         <v>104</v>
       </c>
@@ -11897,7 +11902,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="40" t="s">
         <v>97</v>
       </c>
@@ -11905,7 +11910,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="39" t="s">
         <v>96</v>
       </c>
@@ -11913,7 +11918,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="43" t="s">
         <v>103</v>
       </c>
@@ -11921,7 +11926,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="43" t="s">
         <v>102</v>
       </c>
@@ -11929,7 +11934,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="39" t="s">
         <v>110</v>
       </c>
@@ -11937,7 +11942,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="39" t="s">
         <v>109</v>
       </c>
@@ -11945,7 +11950,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="23.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="43" t="s">
         <v>108</v>
       </c>
@@ -11953,7 +11958,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="42" t="s">
         <v>101</v>
       </c>
@@ -11961,7 +11966,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="45" t="s">
         <v>107</v>
       </c>
@@ -11969,7 +11974,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="46" t="s">
         <v>115</v>
       </c>
@@ -11977,7 +11982,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="46" t="s">
         <v>114</v>
       </c>
@@ -11985,7 +11990,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="42" t="s">
         <v>113</v>
       </c>
@@ -11993,7 +11998,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="46" t="s">
         <v>120</v>
       </c>
@@ -12001,7 +12006,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="44" t="s">
         <v>106</v>
       </c>
@@ -12009,7 +12014,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="44" t="s">
         <v>112</v>
       </c>
@@ -12017,7 +12022,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="44" t="s">
         <v>111</v>
       </c>
@@ -12025,7 +12030,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="47" t="s">
         <v>119</v>
       </c>
@@ -12033,7 +12038,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="44" t="s">
         <v>118</v>
       </c>
@@ -12041,7 +12046,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="44" t="s">
         <v>117</v>
       </c>
@@ -12049,7 +12054,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="12.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="44" t="s">
         <v>116</v>
       </c>

</xml_diff>